<commit_message>
upd. test-11 & datasetprepSD
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-11.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-11.xlsx
@@ -2600,8 +2600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,7 +2887,7 @@
         <v>1.3054860006770495E-2</v>
       </c>
       <c r="T10" s="9">
-        <f t="shared" ref="T10:T15" si="3">(Q10/R10-1) * 100</f>
+        <f t="shared" ref="T10:T14" si="3">(Q10/R10-1) * 100</f>
         <v>21.21116352390866</v>
       </c>
     </row>

</xml_diff>